<commit_message>
antes de los cambios
</commit_message>
<xml_diff>
--- a/Espectro completo de arturo/lista de lineas Arcturus.xlsx
+++ b/Espectro completo de arturo/lista de lineas Arcturus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jessi Dani\OneDrive - Universidad de los andes\Proyecto Teórico\Proyecto-Te-rico-Arturo\Espectro completo de arturo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC56A4F4-EA49-49E4-A786-C4AAA5EC0B17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0C46C28-5A36-47C3-9437-6F53213252F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,23 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
   <si>
     <t>c</t>
   </si>
@@ -101,6 +90,28 @@
   </si>
   <si>
     <t>Selección de líneas de hierro para Arcturus-PEPSI</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Symbol"/>
+        <family val="1"/>
+        <charset val="2"/>
+      </rPr>
+      <t>l</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> aire m</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -457,7 +468,7 @@
   <dimension ref="A1:O1318"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
@@ -559,7 +570,7 @@
         <v>1</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="I8" s="2" t="s">
         <v>0</v>

</xml_diff>